<commit_message>
before fixing order of photo and no photo pages
</commit_message>
<xml_diff>
--- a/targets.xlsx
+++ b/targets.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="14">
   <si>
     <t>p</t>
   </si>
@@ -151,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +176,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -236,7 +248,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -250,12 +262,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent5" xfId="4" builtinId="45"/>
@@ -553,24 +571,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="11"/>
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="G1" s="11" t="s">
+      <c r="E1" s="13"/>
+      <c r="G1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="J1" s="11" t="s">
+      <c r="H1" s="13"/>
+      <c r="J1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="12"/>
+      <c r="K1" s="13"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="13"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -995,44 +1013,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:V37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:O1"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="9.28515625" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="11" width="9.140625" style="4"/>
+    <col min="12" max="12" width="2.85546875" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="10"/>
+      <c r="F1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="I1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="E1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="12"/>
-      <c r="H1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="12"/>
-      <c r="K1" s="11" t="s">
+      <c r="J1" s="11"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="N1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="12"/>
-      <c r="N1" s="11" t="s">
+      <c r="O1" s="13"/>
+      <c r="Q1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="12"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R1" s="13"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>9000</v>
@@ -1040,81 +1063,99 @@
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="1"/>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>100650</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>13800</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>2</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="6">
+        <v>3150</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>2550</v>
+      </c>
+      <c r="R2" s="6"/>
+      <c r="U2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1">
-        <v>100650</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4">
+      <c r="V2" s="11"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>1</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="4">
-        <v>1</v>
-      </c>
-      <c r="K2" s="6">
-        <v>3150</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2" s="4">
-        <v>1</v>
-      </c>
-      <c r="N2" s="6">
-        <v>2550</v>
-      </c>
-      <c r="O2" s="6"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>300</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="4">
+      <c r="D3" s="1"/>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>80550</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>30600</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1">
+        <v>3</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="4">
+        <v>1</v>
+      </c>
+      <c r="N3" s="6">
+        <v>32400</v>
+      </c>
+      <c r="O3" s="6"/>
+      <c r="P3" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>3450</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>2</v>
-      </c>
-      <c r="E3" s="1">
-        <v>80550</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4">
-        <v>2</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="4">
-        <v>2</v>
-      </c>
-      <c r="K3" s="6">
-        <v>32400</v>
-      </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="4">
-        <v>2</v>
-      </c>
-      <c r="N3" s="6">
-        <v>3450</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>3600</v>
@@ -1122,40 +1163,47 @@
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="1"/>
+      <c r="E4" s="4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3600</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="4">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>94050</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="4">
+        <v>2</v>
+      </c>
+      <c r="N4" s="6">
+        <v>35550</v>
+      </c>
+      <c r="O4" s="6"/>
+      <c r="P4" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>40200</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>3</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3600</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="4">
-        <v>3</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="4">
-        <v>3</v>
-      </c>
-      <c r="K4" s="6">
-        <v>35550</v>
-      </c>
-      <c r="L4" s="6"/>
-      <c r="M4" s="4">
-        <v>3</v>
-      </c>
-      <c r="N4" s="6">
-        <v>40200</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>2100</v>
@@ -1163,118 +1211,139 @@
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="1"/>
+      <c r="E5" s="4">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>58500</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="4">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1">
+        <v>58800</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1">
+        <v>2</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="4">
+        <v>3</v>
+      </c>
+      <c r="N5" s="6">
+        <v>8250</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>22650</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>4</v>
-      </c>
-      <c r="E5" s="1">
-        <v>58500</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="4">
-        <v>4</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="4">
-        <v>4</v>
-      </c>
-      <c r="K5" s="6">
-        <v>8250</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="M5" s="4">
-        <v>4</v>
-      </c>
-      <c r="N5" s="6">
-        <v>22650</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>26850</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="4">
+      <c r="D6" s="1"/>
+      <c r="E6" s="4">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>20250</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>4</v>
+      </c>
+      <c r="I6" s="1">
+        <v>37800</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>2</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="4">
+        <v>4</v>
+      </c>
+      <c r="N6" s="6">
+        <v>10200</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P6" s="4">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>7050</v>
+      </c>
+      <c r="R6" s="6"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>5</v>
-      </c>
-      <c r="E6" s="1">
-        <v>20250</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
-        <v>5</v>
-      </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" s="4">
-        <v>5</v>
-      </c>
-      <c r="K6" s="6">
-        <v>10200</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="M6" s="4">
-        <v>5</v>
-      </c>
-      <c r="N6" s="6">
-        <v>7050</v>
-      </c>
-      <c r="O6" s="6"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>6</v>
       </c>
       <c r="B7" s="2">
         <v>46650</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="4">
+      <c r="D7" s="2"/>
+      <c r="E7" s="4">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2">
+        <v>61800</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2">
+        <v>26850</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2">
+        <v>3</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="4">
+        <v>5</v>
+      </c>
+      <c r="N7" s="7">
+        <v>37050</v>
+      </c>
+      <c r="O7" s="7"/>
+      <c r="P7" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>16200</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>6</v>
-      </c>
-      <c r="E7" s="2">
-        <v>61800</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="4">
-        <v>6</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="4">
-        <v>6</v>
-      </c>
-      <c r="K7" s="7">
-        <v>37050</v>
-      </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="4">
-        <v>6</v>
-      </c>
-      <c r="N7" s="7">
-        <v>16200</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>7</v>
       </c>
       <c r="B8" s="2">
         <v>4950</v>
@@ -1282,44 +1351,51 @@
       <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="2"/>
+      <c r="E8" s="4">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2">
+        <v>37200</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>6</v>
+      </c>
+      <c r="I8" s="2">
+        <v>73200</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="4">
+        <v>6</v>
+      </c>
+      <c r="N8" s="7">
+        <v>11400</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="P8" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>8400</v>
+      </c>
+      <c r="R8" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>7</v>
-      </c>
-      <c r="E8" s="2">
-        <v>37200</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4">
-        <v>7</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J8" s="4">
-        <v>7</v>
-      </c>
-      <c r="K8" s="7">
-        <v>11400</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M8" s="4">
-        <v>7</v>
-      </c>
-      <c r="N8" s="7">
-        <v>8400</v>
-      </c>
-      <c r="O8" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>8</v>
       </c>
       <c r="B9" s="2">
         <v>21750</v>
@@ -1327,79 +1403,93 @@
       <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="2"/>
+      <c r="E9" s="4">
+        <v>7</v>
+      </c>
+      <c r="F9" s="2">
+        <v>88500</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>7</v>
+      </c>
+      <c r="I9" s="2">
+        <v>76350</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="4">
+        <v>7</v>
+      </c>
+      <c r="N9" s="7">
+        <v>43500</v>
+      </c>
+      <c r="O9" s="7"/>
+      <c r="P9" s="4">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>18150</v>
+      </c>
+      <c r="R9" s="7"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>8</v>
-      </c>
-      <c r="E9" s="2">
-        <v>88500</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4">
-        <v>8</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="4">
-        <v>8</v>
-      </c>
-      <c r="K9" s="7">
-        <v>43500</v>
-      </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="4">
-        <v>8</v>
-      </c>
-      <c r="N9" s="7">
-        <v>18150</v>
-      </c>
-      <c r="O9" s="7"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>9</v>
       </c>
       <c r="B10" s="2">
         <v>60300</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="4">
+      <c r="D10" s="2"/>
+      <c r="E10" s="4">
+        <v>8</v>
+      </c>
+      <c r="F10" s="2">
+        <v>114300</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>8</v>
+      </c>
+      <c r="I10" s="2">
+        <v>18150</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>2</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="4">
+        <v>8</v>
+      </c>
+      <c r="N10" s="7">
+        <v>15300</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="4">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>11250</v>
+      </c>
+      <c r="R10" s="7"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>9</v>
-      </c>
-      <c r="E10" s="2">
-        <v>114300</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="4">
-        <v>9</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J10" s="4">
-        <v>9</v>
-      </c>
-      <c r="K10" s="7">
-        <v>15300</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M10" s="4">
-        <v>9</v>
-      </c>
-      <c r="N10" s="7">
-        <v>11250</v>
-      </c>
-      <c r="O10" s="7"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>10</v>
       </c>
       <c r="B11" s="2">
         <v>43500</v>
@@ -1407,42 +1497,49 @@
       <c r="C11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="2"/>
+      <c r="E11" s="4">
+        <v>9</v>
+      </c>
+      <c r="F11" s="2">
+        <v>51000</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="4">
+        <v>9</v>
+      </c>
+      <c r="I11" s="2">
+        <v>66900</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>3</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="4">
+        <v>9</v>
+      </c>
+      <c r="N11" s="7">
+        <v>21900</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="P11" s="4">
+        <v>9</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>5400</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>10</v>
-      </c>
-      <c r="E11" s="2">
-        <v>51000</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="4">
-        <v>10</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J11" s="4">
-        <v>10</v>
-      </c>
-      <c r="K11" s="7">
-        <v>21900</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M11" s="4">
-        <v>10</v>
-      </c>
-      <c r="N11" s="7">
-        <v>5400</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>11</v>
       </c>
       <c r="B12" s="3">
         <v>11550</v>
@@ -1450,120 +1547,141 @@
       <c r="C12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3"/>
+      <c r="E12" s="4">
+        <v>10</v>
+      </c>
+      <c r="F12" s="3">
+        <v>138300</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>10</v>
+      </c>
+      <c r="I12" s="3">
+        <v>35400</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="3">
+        <v>1</v>
+      </c>
+      <c r="L12" s="3"/>
+      <c r="M12" s="4">
+        <v>10</v>
+      </c>
+      <c r="N12" s="8">
+        <v>47250</v>
+      </c>
+      <c r="O12" s="8"/>
+      <c r="P12" s="4">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>35850</v>
+      </c>
+      <c r="R12" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>11</v>
-      </c>
-      <c r="E12" s="3">
-        <v>138300</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" s="4">
-        <v>11</v>
-      </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J12" s="4">
-        <v>11</v>
-      </c>
-      <c r="K12" s="8">
-        <v>47250</v>
-      </c>
-      <c r="L12" s="8"/>
-      <c r="M12" s="4">
-        <v>11</v>
-      </c>
-      <c r="N12" s="8">
-        <v>35850</v>
-      </c>
-      <c r="O12" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>12</v>
       </c>
       <c r="B13" s="3">
         <v>34200</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="4">
+      <c r="D13" s="3"/>
+      <c r="E13" s="4">
+        <v>11</v>
+      </c>
+      <c r="F13" s="3">
+        <v>76350</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>11</v>
+      </c>
+      <c r="I13" s="3">
+        <v>43500</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="3">
+        <v>3</v>
+      </c>
+      <c r="L13" s="3"/>
+      <c r="M13" s="4">
+        <v>11</v>
+      </c>
+      <c r="N13" s="8">
+        <v>85500</v>
+      </c>
+      <c r="O13" s="8"/>
+      <c r="P13" s="4">
+        <v>11</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>17400</v>
+      </c>
+      <c r="R13" s="8"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>12</v>
-      </c>
-      <c r="E13" s="3">
-        <v>76350</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G13" s="4">
-        <v>12</v>
-      </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J13" s="4">
-        <v>12</v>
-      </c>
-      <c r="K13" s="8">
-        <v>85500</v>
-      </c>
-      <c r="L13" s="8"/>
-      <c r="M13" s="4">
-        <v>12</v>
-      </c>
-      <c r="N13" s="8">
-        <v>17400</v>
-      </c>
-      <c r="O13" s="8"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>13</v>
       </c>
       <c r="B14" s="3">
         <v>32250</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="4">
+      <c r="D14" s="3"/>
+      <c r="E14" s="4">
+        <v>12</v>
+      </c>
+      <c r="F14" s="15">
+        <v>56850</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="4">
+        <v>12</v>
+      </c>
+      <c r="I14" s="3">
+        <v>24750</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3">
+        <v>2</v>
+      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="4">
+        <v>12</v>
+      </c>
+      <c r="N14" s="8">
+        <v>26250</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="P14" s="4">
+        <v>12</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>10350</v>
+      </c>
+      <c r="R14" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>13</v>
-      </c>
-      <c r="E14" s="3">
-        <v>56850</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="4">
-        <v>13</v>
-      </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="4">
-        <v>13</v>
-      </c>
-      <c r="K14" s="8">
-        <v>26250</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="M14" s="4">
-        <v>13</v>
-      </c>
-      <c r="N14" s="8">
-        <v>10350</v>
-      </c>
-      <c r="O14" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>14</v>
       </c>
       <c r="B15" s="3">
         <v>41850</v>
@@ -1571,40 +1689,47 @@
       <c r="C15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3"/>
+      <c r="E15" s="4">
+        <v>13</v>
+      </c>
+      <c r="F15" s="3">
+        <v>60450</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="4">
+        <v>13</v>
+      </c>
+      <c r="I15" s="3">
+        <v>90150</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3">
+        <v>3</v>
+      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="4">
+        <v>13</v>
+      </c>
+      <c r="N15" s="8">
+        <v>34200</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="P15" s="4">
+        <v>13</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>4650</v>
+      </c>
+      <c r="R15" s="8"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>14</v>
-      </c>
-      <c r="E15" s="3">
-        <v>60450</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4">
-        <v>14</v>
-      </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J15" s="4">
-        <v>14</v>
-      </c>
-      <c r="K15" s="8">
-        <v>34200</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="M15" s="4">
-        <v>14</v>
-      </c>
-      <c r="N15" s="8">
-        <v>4650</v>
-      </c>
-      <c r="O15" s="8"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>15</v>
       </c>
       <c r="B16" s="3">
         <v>138900</v>
@@ -1612,42 +1737,49 @@
       <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3"/>
+      <c r="E16" s="4">
+        <v>14</v>
+      </c>
+      <c r="F16" s="3">
+        <v>78750</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <v>14</v>
+      </c>
+      <c r="I16" s="3">
+        <v>3150</v>
+      </c>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3">
+        <v>1</v>
+      </c>
+      <c r="L16" s="3"/>
+      <c r="M16" s="4">
+        <v>14</v>
+      </c>
+      <c r="N16" s="8">
+        <v>29550</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="P16" s="4">
+        <v>14</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>12300</v>
+      </c>
+      <c r="R16" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
         <v>15</v>
-      </c>
-      <c r="E16" s="3">
-        <v>78750</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G16" s="4">
-        <v>15</v>
-      </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="4">
-        <v>15</v>
-      </c>
-      <c r="K16" s="8">
-        <v>29550</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="M16" s="4">
-        <v>15</v>
-      </c>
-      <c r="N16" s="8">
-        <v>12300</v>
-      </c>
-      <c r="O16" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>16</v>
       </c>
       <c r="B17" s="5">
         <v>85350</v>
@@ -1655,87 +1787,309 @@
       <c r="C17" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="5"/>
+      <c r="E17" s="4">
+        <v>15</v>
+      </c>
+      <c r="F17" s="14">
+        <v>56850</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>15</v>
+      </c>
+      <c r="I17" s="5">
+        <v>27900</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="4">
+        <v>15</v>
+      </c>
+      <c r="N17" s="9">
+        <v>117450</v>
+      </c>
+      <c r="O17" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q17" s="9">
+        <v>41850</v>
+      </c>
+      <c r="R17" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
         <v>16</v>
-      </c>
-      <c r="E17" s="5">
-        <v>56850</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G17" s="4">
-        <v>16</v>
-      </c>
-      <c r="H17" s="5">
-        <v>167700</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J17" s="4">
-        <v>16</v>
-      </c>
-      <c r="K17" s="9">
-        <v>117450</v>
-      </c>
-      <c r="L17" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="M17" s="4">
-        <v>16</v>
-      </c>
-      <c r="N17" s="9">
-        <v>41850</v>
-      </c>
-      <c r="O17" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>17</v>
       </c>
       <c r="B18" s="5">
         <v>88200</v>
       </c>
       <c r="C18" s="5"/>
-      <c r="D18" s="4">
-        <v>17</v>
-      </c>
-      <c r="E18" s="5">
+      <c r="D18" s="5"/>
+      <c r="E18" s="4">
+        <v>16</v>
+      </c>
+      <c r="F18" s="5">
         <v>72000</v>
       </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="4">
-        <v>17</v>
-      </c>
-      <c r="H18" s="5">
-        <v>172950</v>
-      </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="4">
-        <v>17</v>
-      </c>
-      <c r="K18" s="9">
+      <c r="G18" s="5"/>
+      <c r="H18" s="4">
+        <v>16</v>
+      </c>
+      <c r="I18" s="5">
+        <v>87750</v>
+      </c>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="4">
+        <v>16</v>
+      </c>
+      <c r="N18" s="9">
         <v>121050</v>
       </c>
-      <c r="L18" s="9"/>
-      <c r="M18" s="4">
-        <v>17</v>
-      </c>
-      <c r="N18" s="9">
+      <c r="O18" s="9"/>
+      <c r="P18" s="4">
+        <v>16</v>
+      </c>
+      <c r="Q18" s="9">
         <v>45150</v>
       </c>
-      <c r="O18" s="9"/>
+      <c r="R18" s="9"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+      <c r="R22" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E23" s="4">
+        <v>1</v>
+      </c>
+      <c r="P23" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>58.2</v>
+      </c>
+      <c r="R23" s="16">
+        <v>83.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F24" s="4">
+        <v>2</v>
+      </c>
+      <c r="P24" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>116.5</v>
+      </c>
+      <c r="R24" s="4">
+        <v>141.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C25" s="4">
+        <v>3</v>
+      </c>
+      <c r="P25" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>174.8</v>
+      </c>
+      <c r="R25" s="16">
+        <v>199.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E26" s="4">
+        <v>4</v>
+      </c>
+      <c r="P26" s="4">
+        <v>4</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>233.1</v>
+      </c>
+      <c r="R26" s="4">
+        <v>257.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F27" s="4">
+        <v>5</v>
+      </c>
+      <c r="P27" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>291.39999999999998</v>
+      </c>
+      <c r="R27" s="16">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C28" s="4">
+        <v>6</v>
+      </c>
+      <c r="P28" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>349.7</v>
+      </c>
+      <c r="R28" s="4">
+        <v>374.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E29" s="4">
+        <v>7</v>
+      </c>
+      <c r="P29" s="4">
+        <v>7</v>
+      </c>
+      <c r="Q29" s="4">
+        <v>408</v>
+      </c>
+      <c r="R29" s="16">
+        <v>432.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F30" s="4">
+        <v>8</v>
+      </c>
+      <c r="P30" s="4">
+        <v>8</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>466.3</v>
+      </c>
+      <c r="R30" s="4">
+        <v>490.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C31" s="4">
+        <v>9</v>
+      </c>
+      <c r="P31" s="4">
+        <v>9</v>
+      </c>
+      <c r="Q31" s="4">
+        <v>524.6</v>
+      </c>
+      <c r="R31" s="16">
+        <v>548.79999999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E32" s="4">
+        <v>10</v>
+      </c>
+      <c r="P32" s="4">
+        <v>10</v>
+      </c>
+      <c r="Q32" s="4">
+        <v>582.9</v>
+      </c>
+      <c r="R32" s="4">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="33" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="F33" s="4">
+        <v>11</v>
+      </c>
+      <c r="P33" s="4">
+        <v>11</v>
+      </c>
+      <c r="Q33" s="4">
+        <v>641.20000000000005</v>
+      </c>
+      <c r="R33" s="16">
+        <v>665.2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C34" s="4">
+        <v>12</v>
+      </c>
+      <c r="P34" s="4">
+        <v>12</v>
+      </c>
+      <c r="Q34" s="4">
+        <v>699.5</v>
+      </c>
+      <c r="R34" s="4">
+        <v>723.4</v>
+      </c>
+    </row>
+    <row r="35" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="E35" s="4">
+        <v>13</v>
+      </c>
+      <c r="P35" s="4">
+        <v>13</v>
+      </c>
+      <c r="Q35" s="4">
+        <v>757.8</v>
+      </c>
+      <c r="R35" s="16">
+        <v>781.6</v>
+      </c>
+    </row>
+    <row r="36" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="F36" s="4">
+        <v>14</v>
+      </c>
+      <c r="P36" s="4">
+        <v>14</v>
+      </c>
+      <c r="Q36" s="4">
+        <v>816.1</v>
+      </c>
+      <c r="R36" s="4">
+        <v>839.8</v>
+      </c>
+    </row>
+    <row r="37" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="P37" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q37" s="4">
+        <v>874.4</v>
+      </c>
+      <c r="R37" s="16">
+        <v>898</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="U2:V2"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="N1:O1"/>
+    <mergeCell ref="Q1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>